<commit_message>
Added spaces around equal signs
</commit_message>
<xml_diff>
--- a/docs/data/chiropractic_care_table.xlsx
+++ b/docs/data/chiropractic_care_table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\docs\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D98FA3-3A52-4072-89A1-7779981F74D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A768495-9DC1-4806-A382-4C77088F7EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-52110" yWindow="-4830" windowWidth="21600" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,7 +433,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -523,20 +523,6 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B7">
-        <f>SUM(B2:B6)</f>
-        <v>401</v>
-      </c>
-      <c r="C7">
-        <f t="shared" ref="C7:D7" si="0">SUM(C2:C6)</f>
-        <v>481</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>553</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>